<commit_message>
Stacked Column Chart created
I tried to use Mekko chart instead but it seems not to be possible
</commit_message>
<xml_diff>
--- a/BioTables.xlsx
+++ b/BioTables.xlsx
@@ -16,28 +16,28 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C4">
-      <text>
-        <t xml:space="preserve">typical values</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="H4">
+    <comment authorId="0" ref="H1">
       <text>
         <t xml:space="preserve">typical ratio of composition of sea water to living organisms. 
 The greater the value above 1, the more more important it is to sea creatures to seek and store given element</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E5">
+    <comment authorId="0" ref="C2">
+      <text>
+        <t xml:space="preserve">typical values</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E3">
       <text>
         <t xml:space="preserve">oceanic plancton</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F5">
+    <comment authorId="0" ref="F3">
       <text>
         <t xml:space="preserve">estimated average for whole biosphere</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G5">
+    <comment authorId="0" ref="G3">
       <text>
         <t xml:space="preserve">for comparison</t>
       </text>
@@ -47,24 +47,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
-  <si>
-    <t>Elemental Composition of Organisms</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+  <si>
+    <t>Element</t>
   </si>
   <si>
     <t>Chemical Elemenets Content in Living Organisms (w/v)</t>
   </si>
   <si>
-    <t>Element</t>
+    <t>Preconcentration Factor</t>
   </si>
   <si>
     <t>Organisms</t>
   </si>
   <si>
     <t>Other</t>
-  </si>
-  <si>
-    <t>Preconcentration Factor</t>
   </si>
   <si>
     <t>Name</t>
@@ -179,24 +176,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font/>
     <font>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -222,8 +214,24 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -258,6 +266,22 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -269,14 +293,6 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -299,87 +315,77 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="9" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="6" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="8" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -393,6 +399,34 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Chemical Elemenets Content in Living Organisms (w/v)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -403,7 +437,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$5:$B$5</c:f>
+              <c:f>Arkusz1!$A$3:$B$3</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -414,11 +448,74 @@
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:cat>
             <c:strRef>
+              <c:f>Arkusz1!$C$2:$G$2</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$C$3:$G$3</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$A$4:$B$4</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz1!$C$2:$G$2</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
               <c:f>Arkusz1!$C$4:$G$4</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$A$5:$B$5</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz1!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
@@ -429,8 +526,8 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Arkusz1!$A$6:$B$6</c:f>
@@ -438,17 +535,18 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent4"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$4:$G$4</c:f>
+              <c:f>Arkusz1!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
@@ -459,8 +557,8 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="4"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Arkusz1!$A$7:$B$7</c:f>
@@ -468,17 +566,18 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:schemeClr val="accent5"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$4:$G$4</c:f>
+              <c:f>Arkusz1!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
@@ -489,8 +588,8 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:idx val="5"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Arkusz1!$A$8:$B$8</c:f>
@@ -498,17 +597,18 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:schemeClr val="accent6"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$4:$G$4</c:f>
+              <c:f>Arkusz1!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
@@ -519,71 +619,11 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$A$9:$B$9</c:f>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Arkusz1!$C$4:$G$4</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Arkusz1!$C$9:$G$9</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$A$10:$B$10</c:f>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Arkusz1!$C$4:$G$4</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Arkusz1!$C$10:$G$10</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
           <c:idx val="6"/>
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$11:$B$11</c:f>
+              <c:f>Arkusz1!$A$9:$B$9</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -596,16 +636,17 @@
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$4:$G$4</c:f>
+              <c:f>Arkusz1!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$11:$G$11</c:f>
+              <c:f>Arkusz1!$C$9:$G$9</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -615,7 +656,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$12:$B$12</c:f>
+              <c:f>Arkusz1!$A$10:$B$10</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -628,16 +669,17 @@
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$4:$G$4</c:f>
+              <c:f>Arkusz1!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$12:$G$12</c:f>
+              <c:f>Arkusz1!$C$10:$G$10</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -647,7 +689,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$13:$B$13</c:f>
+              <c:f>Arkusz1!$A$11:$B$11</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -660,16 +702,17 @@
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$4:$G$4</c:f>
+              <c:f>Arkusz1!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$13:$G$13</c:f>
+              <c:f>Arkusz1!$C$11:$G$11</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -679,7 +722,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$14:$B$14</c:f>
+              <c:f>Arkusz1!$A$12:$B$12</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -692,16 +735,17 @@
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$4:$G$4</c:f>
+              <c:f>Arkusz1!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$14:$G$14</c:f>
+              <c:f>Arkusz1!$C$12:$G$12</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -711,7 +755,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$15:$B$15</c:f>
+              <c:f>Arkusz1!$A$13:$B$13</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -724,16 +768,17 @@
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$4:$G$4</c:f>
+              <c:f>Arkusz1!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$15:$G$15</c:f>
+              <c:f>Arkusz1!$C$13:$G$13</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -743,7 +788,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$16:$B$16</c:f>
+              <c:f>Arkusz1!$A$14:$B$14</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -756,16 +801,17 @@
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$4:$G$4</c:f>
+              <c:f>Arkusz1!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$16:$G$16</c:f>
+              <c:f>Arkusz1!$C$14:$G$14</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -775,7 +821,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$17:$B$17</c:f>
+              <c:f>Arkusz1!$A$15:$B$15</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -788,16 +834,17 @@
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$4:$G$4</c:f>
+              <c:f>Arkusz1!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$17:$G$17</c:f>
+              <c:f>Arkusz1!$C$15:$G$15</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -807,7 +854,7 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$18:$B$18</c:f>
+              <c:f>Arkusz1!$A$16:$B$16</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -820,16 +867,17 @@
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$4:$G$4</c:f>
+              <c:f>Arkusz1!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$18:$G$18</c:f>
+              <c:f>Arkusz1!$C$16:$G$16</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -839,27 +887,27 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$19:$B$19</c:f>
+              <c:f>Arkusz1!$A$17:$B$17</c:f>
             </c:strRef>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$4:$G$4</c:f>
+              <c:f>Arkusz1!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$19:$G$19</c:f>
+              <c:f>Arkusz1!$C$17:$G$17</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1636625622"/>
-        <c:axId val="484511391"/>
+        <c:axId val="1952170857"/>
+        <c:axId val="1853141930"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1636625622"/>
+        <c:axId val="1952170857"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -902,7 +950,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0">
+              <a:defRPr b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -911,35 +959,15 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="484511391"/>
+        <c:crossAx val="1853141930"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="484511391"/>
+        <c:axId val="1853141930"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="CCCCCC">
-                  <a:alpha val="0"/>
-                </a:srgbClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -989,7 +1017,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1636625622"/>
+        <c:crossAx val="1952170857"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1022,7 +1050,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
@@ -1062,28 +1090,28 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="5891AD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="004561"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="FF6F31"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="1C7685"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="0F45A8"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="4CDC8B"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0097A7"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0097A7"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
@@ -1258,433 +1286,427 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
+      <c r="A3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="17"/>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="9" t="s">
-        <v>5</v>
+      <c r="A4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="20">
+        <v>61.0</v>
+      </c>
+      <c r="D4" s="21">
+        <v>67.9</v>
+      </c>
+      <c r="E4" s="21">
+        <v>80.0</v>
+      </c>
+      <c r="F4" s="21">
+        <v>70.0</v>
+      </c>
+      <c r="G4" s="21">
+        <v>85.9</v>
+      </c>
+      <c r="H4" s="21">
+        <v>0.8</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="15"/>
+      <c r="A5" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="20">
+        <v>23.0</v>
+      </c>
+      <c r="D5" s="21">
+        <v>11.3</v>
+      </c>
+      <c r="E5" s="21">
+        <v>6.1</v>
+      </c>
+      <c r="F5" s="21">
+        <v>18.0</v>
+      </c>
+      <c r="G5" s="21">
+        <v>0.028</v>
+      </c>
+      <c r="H5" s="21">
+        <v>640.0</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="18">
-        <v>61.0</v>
-      </c>
-      <c r="D6" s="19">
-        <v>67.9</v>
-      </c>
-      <c r="E6" s="19">
-        <v>80.0</v>
-      </c>
-      <c r="F6" s="19">
-        <v>70.0</v>
-      </c>
-      <c r="G6" s="19">
-        <v>85.9</v>
-      </c>
-      <c r="H6" s="19">
-        <v>0.8</v>
+      <c r="A6" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="20">
+        <v>10.0</v>
+      </c>
+      <c r="D6" s="21">
+        <v>8.72</v>
+      </c>
+      <c r="E6" s="21">
+        <v>10.2</v>
+      </c>
+      <c r="F6" s="21">
+        <v>15.5</v>
+      </c>
+      <c r="G6" s="22">
+        <v>10.8</v>
+      </c>
+      <c r="H6" s="21">
+        <v>1.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="18">
-        <v>23.0</v>
-      </c>
-      <c r="D7" s="19">
-        <v>11.3</v>
-      </c>
-      <c r="E7" s="19">
-        <v>6.1</v>
-      </c>
-      <c r="F7" s="19">
-        <v>18.0</v>
-      </c>
-      <c r="G7" s="19">
-        <v>0.028</v>
-      </c>
-      <c r="H7" s="19">
-        <v>640.0</v>
+      <c r="A7" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="20">
+        <v>2.6</v>
+      </c>
+      <c r="D7" s="21">
+        <v>8.25</v>
+      </c>
+      <c r="E7" s="21">
+        <v>1.52</v>
+      </c>
+      <c r="F7" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="G7" s="21">
+        <v>5.0E-5</v>
+      </c>
+      <c r="H7" s="21">
+        <v>6000.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="18">
-        <v>10.0</v>
-      </c>
-      <c r="D8" s="19">
-        <v>8.72</v>
-      </c>
-      <c r="E8" s="19">
-        <v>10.2</v>
-      </c>
-      <c r="F8" s="19">
-        <v>15.5</v>
-      </c>
-      <c r="G8" s="20">
-        <v>10.8</v>
-      </c>
-      <c r="H8" s="19">
-        <v>1.0</v>
+      <c r="A8" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="20">
+        <v>1.4</v>
+      </c>
+      <c r="D8" s="21">
+        <v>0.58</v>
+      </c>
+      <c r="E8" s="21">
+        <v>0.04</v>
+      </c>
+      <c r="F8" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="G8" s="21">
+        <v>0.0408</v>
+      </c>
+      <c r="H8" s="21">
+        <v>7.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="18">
-        <v>2.6</v>
-      </c>
-      <c r="D9" s="19">
-        <v>8.25</v>
-      </c>
-      <c r="E9" s="19">
-        <v>1.52</v>
-      </c>
-      <c r="F9" s="19">
-        <v>0.3</v>
-      </c>
-      <c r="G9" s="19">
-        <v>5.0E-5</v>
-      </c>
-      <c r="H9" s="19">
-        <v>6000.0</v>
+      <c r="A9" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="20">
+        <v>1.1</v>
+      </c>
+      <c r="D9" s="21">
+        <v>0.71</v>
+      </c>
+      <c r="E9" s="21">
+        <v>0.13</v>
+      </c>
+      <c r="F9" s="21">
+        <v>0.07</v>
+      </c>
+      <c r="G9" s="21">
+        <v>7.0E-6</v>
+      </c>
+      <c r="H9" s="21">
+        <v>10000.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="18">
-        <v>1.4</v>
-      </c>
-      <c r="D10" s="19">
-        <v>0.58</v>
-      </c>
-      <c r="E10" s="19">
-        <v>0.04</v>
-      </c>
-      <c r="F10" s="19">
-        <v>0.3</v>
-      </c>
-      <c r="G10" s="19">
-        <v>0.0408</v>
-      </c>
-      <c r="H10" s="19">
-        <v>7.0</v>
+      <c r="A10" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="D10" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="E10" s="21">
+        <v>0.14</v>
+      </c>
+      <c r="F10" s="21">
+        <v>0.05</v>
+      </c>
+      <c r="G10" s="21">
+        <v>0.09</v>
+      </c>
+      <c r="H10" s="21">
+        <v>0.4</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="18">
-        <v>1.1</v>
-      </c>
-      <c r="D11" s="19">
-        <v>0.71</v>
-      </c>
-      <c r="E11" s="19">
-        <v>0.13</v>
-      </c>
-      <c r="F11" s="19">
-        <v>0.07</v>
-      </c>
-      <c r="G11" s="19">
-        <v>7.0E-6</v>
-      </c>
-      <c r="H11" s="19">
-        <v>10000.0</v>
+      <c r="A11" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="20">
+        <v>0.14</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="21">
+        <v>0.54</v>
+      </c>
+      <c r="F11" s="21">
+        <v>0.02</v>
+      </c>
+      <c r="G11" s="21">
+        <v>1.08</v>
+      </c>
+      <c r="H11" s="21">
+        <v>0.02</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="18">
-        <v>0.2</v>
-      </c>
-      <c r="D12" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="E12" s="19">
-        <v>0.14</v>
-      </c>
-      <c r="F12" s="19">
-        <v>0.05</v>
-      </c>
-      <c r="G12" s="19">
-        <v>0.09</v>
-      </c>
-      <c r="H12" s="19">
-        <v>0.4</v>
+      <c r="A12" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="20">
+        <v>0.12</v>
+      </c>
+      <c r="D12" s="21">
+        <v>0.17</v>
+      </c>
+      <c r="E12" s="21">
+        <v>0.29</v>
+      </c>
+      <c r="F12" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="G12" s="21">
+        <v>0.039</v>
+      </c>
+      <c r="H12" s="21">
+        <v>8.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="18">
-        <v>0.14</v>
-      </c>
-      <c r="D13" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="E13" s="19">
-        <v>0.54</v>
-      </c>
-      <c r="F13" s="19">
+      <c r="A13" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="20">
+        <v>0.12</v>
+      </c>
+      <c r="D13" s="21">
+        <v>0.07</v>
+      </c>
+      <c r="E13" s="21">
+        <v>1.05</v>
+      </c>
+      <c r="F13" s="21">
         <v>0.02</v>
       </c>
-      <c r="G13" s="19">
-        <v>1.08</v>
-      </c>
-      <c r="H13" s="19">
-        <v>0.02</v>
+      <c r="G13" s="21">
+        <v>1.935</v>
+      </c>
+      <c r="H13" s="21">
+        <v>0.01</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="18">
-        <v>0.12</v>
-      </c>
-      <c r="D14" s="19">
-        <v>0.17</v>
-      </c>
-      <c r="E14" s="19">
-        <v>0.29</v>
-      </c>
-      <c r="F14" s="19">
+      <c r="A14" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="D14" s="21">
+        <v>0.082</v>
+      </c>
+      <c r="E14" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="F14" s="21">
+        <v>0.04</v>
+      </c>
+      <c r="G14" s="21">
+        <v>0.13</v>
+      </c>
+      <c r="H14" s="21">
         <v>0.3</v>
-      </c>
-      <c r="G14" s="19">
-        <v>0.039</v>
-      </c>
-      <c r="H14" s="19">
-        <v>8.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="18">
-        <v>0.12</v>
-      </c>
-      <c r="D15" s="19">
-        <v>0.07</v>
-      </c>
-      <c r="E15" s="19">
-        <v>1.05</v>
-      </c>
-      <c r="F15" s="19">
-        <v>0.02</v>
-      </c>
-      <c r="G15" s="19">
-        <v>1.935</v>
-      </c>
-      <c r="H15" s="19">
+      <c r="A15" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="20">
+        <v>0.006</v>
+      </c>
+      <c r="D15" s="21">
+        <v>0.0027</v>
+      </c>
+      <c r="E15" s="21">
+        <v>0.007</v>
+      </c>
+      <c r="F15" s="21">
         <v>0.01</v>
+      </c>
+      <c r="G15" s="21">
+        <v>1.0E-6</v>
+      </c>
+      <c r="H15" s="21">
+        <v>10000.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="18">
-        <v>0.03</v>
-      </c>
-      <c r="D16" s="19">
-        <v>0.082</v>
-      </c>
-      <c r="E16" s="19">
-        <v>0.03</v>
-      </c>
-      <c r="F16" s="19">
-        <v>0.04</v>
-      </c>
-      <c r="G16" s="19">
-        <v>0.13</v>
-      </c>
-      <c r="H16" s="19">
-        <v>0.3</v>
+      <c r="A16" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="20">
+        <v>0.0033</v>
+      </c>
+      <c r="D16" s="21">
+        <v>4.0E-4</v>
+      </c>
+      <c r="E16" s="21">
+        <v>4.0E-4</v>
+      </c>
+      <c r="F16" s="21">
+        <v>3.0E-4</v>
+      </c>
+      <c r="G16" s="21">
+        <v>1.0E-6</v>
+      </c>
+      <c r="H16" s="21">
+        <v>300.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="18">
-        <v>0.006</v>
-      </c>
-      <c r="D17" s="19">
-        <v>0.0027</v>
-      </c>
-      <c r="E17" s="19">
+      <c r="A17" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="25">
+        <v>0.0026</v>
+      </c>
+      <c r="D17" s="26">
+        <v>0.0093</v>
+      </c>
+      <c r="E17" s="26">
         <v>0.007</v>
       </c>
-      <c r="F17" s="19">
-        <v>0.01</v>
-      </c>
-      <c r="G17" s="19">
-        <v>1.0E-6</v>
-      </c>
-      <c r="H17" s="19">
-        <v>10000.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="18">
-        <v>0.0033</v>
-      </c>
-      <c r="D18" s="19">
-        <v>4.0E-4</v>
-      </c>
-      <c r="E18" s="19">
-        <v>4.0E-4</v>
-      </c>
-      <c r="F18" s="19">
+      <c r="F17" s="26">
+        <v>0.2</v>
+      </c>
+      <c r="G17" s="26">
         <v>3.0E-4</v>
       </c>
-      <c r="G18" s="19">
-        <v>1.0E-6</v>
-      </c>
-      <c r="H18" s="19">
-        <v>300.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="23">
-        <v>0.0026</v>
-      </c>
-      <c r="D19" s="24">
-        <v>0.0093</v>
-      </c>
-      <c r="E19" s="24">
-        <v>0.007</v>
-      </c>
-      <c r="F19" s="24">
-        <v>0.2</v>
-      </c>
-      <c r="G19" s="24">
-        <v>3.0E-4</v>
-      </c>
-      <c r="H19" s="24">
+      <c r="H17" s="26">
         <v>670.0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="F4:G4"/>
+  <mergeCells count="5">
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="H1:H3"/>
   </mergeCells>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>

<commit_message>
Added new spreadsheet for raw data only
</commit_message>
<xml_diff>
--- a/BioTables.xlsx
+++ b/BioTables.xlsx
@@ -3,9 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Arkusz1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="DB" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Table 1" sheetId="2" r:id="rId5"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="ChemCompOrganisms">DB!$A$1:$H$15</definedName>
+  </definedNames>
   <calcPr/>
 </workbook>
 </file>
@@ -47,7 +50,115 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Lucerne</t>
+  </si>
+  <si>
+    <t>Crustacean</t>
+  </si>
+  <si>
+    <t>Biosphere</t>
+  </si>
+  <si>
+    <t>Oceanic Water</t>
+  </si>
+  <si>
+    <t>Preconcentration Factor</t>
+  </si>
+  <si>
+    <t>Oxygen</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Carbon</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Nitrogen</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Calcium</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>Phosphor</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Sulfur</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Sodium</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>Potassium</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Chlorine</t>
+  </si>
+  <si>
+    <t>Cl</t>
+  </si>
+  <si>
+    <t>Magnessium</t>
+  </si>
+  <si>
+    <t>Mg</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>Fe</t>
+  </si>
+  <si>
+    <t>Zinc</t>
+  </si>
+  <si>
+    <t>Zn</t>
+  </si>
+  <si>
+    <t>Silicone</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
   <si>
     <t>Element</t>
   </si>
@@ -55,118 +166,10 @@
     <t>Chemical Elemenets Content in Living Organisms (w/v)</t>
   </si>
   <si>
-    <t>Preconcentration Factor</t>
-  </si>
-  <si>
     <t>Organisms</t>
   </si>
   <si>
     <t>Other</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Symbol</t>
-  </si>
-  <si>
-    <t>Human</t>
-  </si>
-  <si>
-    <t>Lucerne</t>
-  </si>
-  <si>
-    <t>Crustacean</t>
-  </si>
-  <si>
-    <t>Biosphere</t>
-  </si>
-  <si>
-    <t>Oceanic Water</t>
-  </si>
-  <si>
-    <t>Oxygen</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>Carbon</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Hydrogen</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>Nitrogen</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Calcium</t>
-  </si>
-  <si>
-    <t>Ca</t>
-  </si>
-  <si>
-    <t>Phosphor</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>Sulfur</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Sodium</t>
-  </si>
-  <si>
-    <t>Na</t>
-  </si>
-  <si>
-    <t>Potassium</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>Chlorine</t>
-  </si>
-  <si>
-    <t>Cl</t>
-  </si>
-  <si>
-    <t>Magnessium</t>
-  </si>
-  <si>
-    <t>Mg</t>
-  </si>
-  <si>
-    <t>Iron</t>
-  </si>
-  <si>
-    <t>Fe</t>
-  </si>
-  <si>
-    <t>Zinc</t>
-  </si>
-  <si>
-    <t>Zn</t>
-  </si>
-  <si>
-    <t>Silicone</t>
-  </si>
-  <si>
-    <t>Si</t>
   </si>
 </sst>
 </file>
@@ -182,11 +185,15 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Docs-Roboto"/>
+    </font>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -194,10 +201,6 @@
     <font>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
-    </font>
-    <font>
-      <color rgb="FF000000"/>
-      <name val="Docs-Roboto"/>
     </font>
   </fonts>
   <fills count="3">
@@ -214,8 +217,65 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border/>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -252,140 +312,117 @@
       </bottom>
     </border>
     <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="38">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="9" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="9" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="9" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="2" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="6" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="10" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -437,7 +474,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$3:$B$3</c:f>
+              <c:f>'Table 1'!$A$3:$B$3</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -453,12 +490,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$2:$G$2</c:f>
+              <c:f>'Table 1'!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$3:$G$3</c:f>
+              <c:f>'Table 1'!$C$3:$G$3</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -468,7 +505,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$4:$B$4</c:f>
+              <c:f>'Table 1'!$A$4:$B$4</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -484,12 +521,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$2:$G$2</c:f>
+              <c:f>'Table 1'!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$4:$G$4</c:f>
+              <c:f>'Table 1'!$C$4:$G$4</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -499,7 +536,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$5:$B$5</c:f>
+              <c:f>'Table 1'!$A$5:$B$5</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -515,12 +552,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$2:$G$2</c:f>
+              <c:f>'Table 1'!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$5:$G$5</c:f>
+              <c:f>'Table 1'!$C$5:$G$5</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -530,7 +567,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$6:$B$6</c:f>
+              <c:f>'Table 1'!$A$6:$B$6</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -546,12 +583,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$2:$G$2</c:f>
+              <c:f>'Table 1'!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$6:$G$6</c:f>
+              <c:f>'Table 1'!$C$6:$G$6</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -561,7 +598,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$7:$B$7</c:f>
+              <c:f>'Table 1'!$A$7:$B$7</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -577,12 +614,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$2:$G$2</c:f>
+              <c:f>'Table 1'!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$7:$G$7</c:f>
+              <c:f>'Table 1'!$C$7:$G$7</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -592,7 +629,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$8:$B$8</c:f>
+              <c:f>'Table 1'!$A$8:$B$8</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -608,12 +645,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$2:$G$2</c:f>
+              <c:f>'Table 1'!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$8:$G$8</c:f>
+              <c:f>'Table 1'!$C$8:$G$8</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -623,7 +660,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$9:$B$9</c:f>
+              <c:f>'Table 1'!$A$9:$B$9</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -641,12 +678,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$2:$G$2</c:f>
+              <c:f>'Table 1'!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$9:$G$9</c:f>
+              <c:f>'Table 1'!$C$9:$G$9</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -656,7 +693,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$10:$B$10</c:f>
+              <c:f>'Table 1'!$A$10:$B$10</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -674,12 +711,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$2:$G$2</c:f>
+              <c:f>'Table 1'!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$10:$G$10</c:f>
+              <c:f>'Table 1'!$C$10:$G$10</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -689,7 +726,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$11:$B$11</c:f>
+              <c:f>'Table 1'!$A$11:$B$11</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -707,12 +744,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$2:$G$2</c:f>
+              <c:f>'Table 1'!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$11:$G$11</c:f>
+              <c:f>'Table 1'!$C$11:$G$11</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -722,7 +759,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$12:$B$12</c:f>
+              <c:f>'Table 1'!$A$12:$B$12</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -740,12 +777,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$2:$G$2</c:f>
+              <c:f>'Table 1'!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$12:$G$12</c:f>
+              <c:f>'Table 1'!$C$12:$G$12</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -755,7 +792,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$13:$B$13</c:f>
+              <c:f>'Table 1'!$A$13:$B$13</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -773,12 +810,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$2:$G$2</c:f>
+              <c:f>'Table 1'!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$13:$G$13</c:f>
+              <c:f>'Table 1'!$C$13:$G$13</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -788,7 +825,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$14:$B$14</c:f>
+              <c:f>'Table 1'!$A$14:$B$14</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -806,12 +843,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$2:$G$2</c:f>
+              <c:f>'Table 1'!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$14:$G$14</c:f>
+              <c:f>'Table 1'!$C$14:$G$14</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -821,7 +858,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$15:$B$15</c:f>
+              <c:f>'Table 1'!$A$15:$B$15</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -839,12 +876,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$2:$G$2</c:f>
+              <c:f>'Table 1'!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$15:$G$15</c:f>
+              <c:f>'Table 1'!$C$15:$G$15</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -854,7 +891,7 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$16:$B$16</c:f>
+              <c:f>'Table 1'!$A$16:$B$16</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -872,12 +909,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$2:$G$2</c:f>
+              <c:f>'Table 1'!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$16:$G$16</c:f>
+              <c:f>'Table 1'!$C$16:$G$16</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -887,27 +924,27 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$17:$B$17</c:f>
+              <c:f>'Table 1'!$A$17:$B$17</c:f>
             </c:strRef>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$2:$G$2</c:f>
+              <c:f>'Table 1'!$C$2:$G$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$17:$G$17</c:f>
+              <c:f>'Table 1'!$C$17:$G$17</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1952170857"/>
-        <c:axId val="1853141930"/>
+        <c:axId val="923394000"/>
+        <c:axId val="847275422"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1952170857"/>
+        <c:axId val="923394000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -959,10 +996,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1853141930"/>
+        <c:crossAx val="847275422"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1853141930"/>
+        <c:axId val="847275422"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1017,7 +1054,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1952170857"/>
+        <c:crossAx val="923394000"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1044,6 +1081,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -1277,436 +1318,847 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="12.0"/>
+    <col customWidth="1" min="2" max="2" width="7.43"/>
+    <col customWidth="1" min="8" max="8" width="16.14"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="9">
+        <v>61.0</v>
+      </c>
+      <c r="D2" s="10">
+        <v>67.9</v>
+      </c>
+      <c r="E2" s="10">
+        <v>80.0</v>
+      </c>
+      <c r="F2" s="10">
+        <v>70.0</v>
+      </c>
+      <c r="G2" s="10">
+        <v>85.9</v>
+      </c>
+      <c r="H2" s="10">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="9">
+        <v>23.0</v>
+      </c>
+      <c r="D3" s="10">
+        <v>11.3</v>
+      </c>
+      <c r="E3" s="10">
+        <v>6.1</v>
+      </c>
+      <c r="F3" s="10">
+        <v>18.0</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0.028</v>
+      </c>
+      <c r="H3" s="10">
+        <v>640.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="9">
+        <v>10.0</v>
+      </c>
+      <c r="D4" s="11">
+        <v>8.72</v>
+      </c>
+      <c r="E4" s="11">
+        <v>10.2</v>
+      </c>
+      <c r="F4" s="11">
+        <v>15.5</v>
+      </c>
+      <c r="G4" s="12">
+        <v>10.8</v>
+      </c>
+      <c r="H4" s="11">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9">
+        <v>2.6</v>
+      </c>
+      <c r="D5" s="10">
+        <v>8.25</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1.52</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G5" s="10">
+        <v>5.0E-5</v>
+      </c>
+      <c r="H5" s="10">
+        <v>6000.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1.4</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.58</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0.0408</v>
+      </c>
+      <c r="H6" s="10">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1.1</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.71</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0.13</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.07</v>
+      </c>
+      <c r="G7" s="10">
+        <v>7.0E-6</v>
+      </c>
+      <c r="H7" s="10">
+        <v>10000.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0.14</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0.09</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0.14</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.54</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="G9" s="10">
+        <v>1.08</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.17</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.29</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0.039</v>
+      </c>
+      <c r="H10" s="10">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.07</v>
+      </c>
+      <c r="E11" s="10">
+        <v>1.05</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="G11" s="10">
+        <v>1.935</v>
+      </c>
+      <c r="H11" s="10">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0.082</v>
+      </c>
+      <c r="E12" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0.13</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.006</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.0027</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0.007</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="G13" s="10">
+        <v>1.0E-6</v>
+      </c>
+      <c r="H13" s="10">
+        <v>10000.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.0033</v>
+      </c>
+      <c r="D14" s="10">
+        <v>4.0E-4</v>
+      </c>
+      <c r="E14" s="10">
+        <v>4.0E-4</v>
+      </c>
+      <c r="F14" s="10">
+        <v>3.0E-4</v>
+      </c>
+      <c r="G14" s="10">
+        <v>1.0E-6</v>
+      </c>
+      <c r="H14" s="10">
+        <v>300.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="15">
+        <v>0.0026</v>
+      </c>
+      <c r="D15" s="16">
+        <v>0.0093</v>
+      </c>
+      <c r="E15" s="16">
+        <v>0.007</v>
+      </c>
+      <c r="F15" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="G15" s="16">
+        <v>3.0E-4</v>
+      </c>
+      <c r="H15" s="16">
+        <v>670.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
     <col customWidth="1" min="2" max="2" width="7.43"/>
     <col customWidth="1" min="5" max="5" width="14.86"/>
     <col customWidth="1" min="8" max="8" width="15.57"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
+      <c r="A1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="27"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="28" t="str">
+        <f t="array" ref="A3:H17">ChemCompOrganisms</f>
+        <v>Name</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="6" t="s">
+      <c r="C3" s="29" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9" t="s">
+      <c r="D3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="10" t="s">
+      <c r="E3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="11"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="12" t="s">
+      <c r="F3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="G3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="H3" s="32"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="B4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="C4" s="9">
+        <v>61.0</v>
+      </c>
+      <c r="D4" s="10">
+        <v>67.9</v>
+      </c>
+      <c r="E4" s="10">
+        <v>80.0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>70.0</v>
+      </c>
+      <c r="G4" s="10">
+        <v>85.9</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="B5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="17"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="18" t="s">
+      <c r="C5" s="9">
+        <v>23.0</v>
+      </c>
+      <c r="D5" s="10">
+        <v>11.3</v>
+      </c>
+      <c r="E5" s="10">
+        <v>6.1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>18.0</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0.028</v>
+      </c>
+      <c r="H5" s="10">
+        <v>640.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B6" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="20">
-        <v>61.0</v>
-      </c>
-      <c r="D4" s="21">
-        <v>67.9</v>
-      </c>
-      <c r="E4" s="21">
-        <v>80.0</v>
-      </c>
-      <c r="F4" s="21">
-        <v>70.0</v>
-      </c>
-      <c r="G4" s="21">
-        <v>85.9</v>
-      </c>
-      <c r="H4" s="21">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="18" t="s">
+      <c r="C6" s="9">
+        <v>10.0</v>
+      </c>
+      <c r="D6" s="10">
+        <v>8.72</v>
+      </c>
+      <c r="E6" s="10">
+        <v>10.2</v>
+      </c>
+      <c r="F6" s="10">
+        <v>15.5</v>
+      </c>
+      <c r="G6" s="35">
+        <v>10.8</v>
+      </c>
+      <c r="H6" s="10">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B7" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="20">
-        <v>23.0</v>
-      </c>
-      <c r="D5" s="21">
-        <v>11.3</v>
-      </c>
-      <c r="E5" s="21">
-        <v>6.1</v>
-      </c>
-      <c r="F5" s="21">
-        <v>18.0</v>
-      </c>
-      <c r="G5" s="21">
-        <v>0.028</v>
-      </c>
-      <c r="H5" s="21">
-        <v>640.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="18" t="s">
+      <c r="C7" s="9">
+        <v>2.6</v>
+      </c>
+      <c r="D7" s="10">
+        <v>8.25</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1.52</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G7" s="10">
+        <v>5.0E-5</v>
+      </c>
+      <c r="H7" s="10">
+        <v>6000.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B8" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="20">
-        <v>10.0</v>
-      </c>
-      <c r="D6" s="21">
-        <v>8.72</v>
-      </c>
-      <c r="E6" s="21">
-        <v>10.2</v>
-      </c>
-      <c r="F6" s="21">
-        <v>15.5</v>
-      </c>
-      <c r="G6" s="22">
-        <v>10.8</v>
-      </c>
-      <c r="H6" s="21">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="18" t="s">
+      <c r="C8" s="9">
+        <v>1.4</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.58</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0.0408</v>
+      </c>
+      <c r="H8" s="10">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B9" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="20">
-        <v>2.6</v>
-      </c>
-      <c r="D7" s="21">
-        <v>8.25</v>
-      </c>
-      <c r="E7" s="21">
-        <v>1.52</v>
-      </c>
-      <c r="F7" s="21">
+      <c r="C9" s="9">
+        <v>1.1</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.71</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.13</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.07</v>
+      </c>
+      <c r="G9" s="10">
+        <v>7.0E-6</v>
+      </c>
+      <c r="H9" s="10">
+        <v>10000.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.14</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0.09</v>
+      </c>
+      <c r="H10" s="10">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.14</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0.54</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="G11" s="10">
+        <v>1.08</v>
+      </c>
+      <c r="H11" s="10">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0.17</v>
+      </c>
+      <c r="E12" s="10">
+        <v>0.29</v>
+      </c>
+      <c r="F12" s="10">
         <v>0.3</v>
       </c>
-      <c r="G7" s="21">
-        <v>5.0E-5</v>
-      </c>
-      <c r="H7" s="21">
-        <v>6000.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="20">
-        <v>1.4</v>
-      </c>
-      <c r="D8" s="21">
-        <v>0.58</v>
-      </c>
-      <c r="E8" s="21">
+      <c r="G12" s="10">
+        <v>0.039</v>
+      </c>
+      <c r="H12" s="10">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.07</v>
+      </c>
+      <c r="E13" s="10">
+        <v>1.05</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="G13" s="10">
+        <v>1.935</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0.082</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="F14" s="10">
         <v>0.04</v>
       </c>
-      <c r="F8" s="21">
+      <c r="G14" s="10">
+        <v>0.13</v>
+      </c>
+      <c r="H14" s="10">
         <v>0.3</v>
       </c>
-      <c r="G8" s="21">
-        <v>0.0408</v>
-      </c>
-      <c r="H8" s="21">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="20">
-        <v>1.1</v>
-      </c>
-      <c r="D9" s="21">
-        <v>0.71</v>
-      </c>
-      <c r="E9" s="21">
-        <v>0.13</v>
-      </c>
-      <c r="F9" s="21">
-        <v>0.07</v>
-      </c>
-      <c r="G9" s="21">
-        <v>7.0E-6</v>
-      </c>
-      <c r="H9" s="21">
+    </row>
+    <row r="15">
+      <c r="A15" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0.006</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0.0027</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0.007</v>
+      </c>
+      <c r="F15" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="G15" s="10">
+        <v>1.0E-6</v>
+      </c>
+      <c r="H15" s="10">
         <v>10000.0</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="20">
+    <row r="16">
+      <c r="A16" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.0033</v>
+      </c>
+      <c r="D16" s="10">
+        <v>4.0E-4</v>
+      </c>
+      <c r="E16" s="10">
+        <v>4.0E-4</v>
+      </c>
+      <c r="F16" s="10">
+        <v>3.0E-4</v>
+      </c>
+      <c r="G16" s="10">
+        <v>1.0E-6</v>
+      </c>
+      <c r="H16" s="10">
+        <v>300.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="15">
+        <v>0.0026</v>
+      </c>
+      <c r="D17" s="16">
+        <v>0.0093</v>
+      </c>
+      <c r="E17" s="16">
+        <v>0.007</v>
+      </c>
+      <c r="F17" s="16">
         <v>0.2</v>
       </c>
-      <c r="D10" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="E10" s="21">
-        <v>0.14</v>
-      </c>
-      <c r="F10" s="21">
-        <v>0.05</v>
-      </c>
-      <c r="G10" s="21">
-        <v>0.09</v>
-      </c>
-      <c r="H10" s="21">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="20">
-        <v>0.14</v>
-      </c>
-      <c r="D11" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="E11" s="21">
-        <v>0.54</v>
-      </c>
-      <c r="F11" s="21">
-        <v>0.02</v>
-      </c>
-      <c r="G11" s="21">
-        <v>1.08</v>
-      </c>
-      <c r="H11" s="21">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="20">
-        <v>0.12</v>
-      </c>
-      <c r="D12" s="21">
-        <v>0.17</v>
-      </c>
-      <c r="E12" s="21">
-        <v>0.29</v>
-      </c>
-      <c r="F12" s="21">
-        <v>0.3</v>
-      </c>
-      <c r="G12" s="21">
-        <v>0.039</v>
-      </c>
-      <c r="H12" s="21">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="20">
-        <v>0.12</v>
-      </c>
-      <c r="D13" s="21">
-        <v>0.07</v>
-      </c>
-      <c r="E13" s="21">
-        <v>1.05</v>
-      </c>
-      <c r="F13" s="21">
-        <v>0.02</v>
-      </c>
-      <c r="G13" s="21">
-        <v>1.935</v>
-      </c>
-      <c r="H13" s="21">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="D14" s="21">
-        <v>0.082</v>
-      </c>
-      <c r="E14" s="21">
-        <v>0.03</v>
-      </c>
-      <c r="F14" s="21">
-        <v>0.04</v>
-      </c>
-      <c r="G14" s="21">
-        <v>0.13</v>
-      </c>
-      <c r="H14" s="21">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="20">
-        <v>0.006</v>
-      </c>
-      <c r="D15" s="21">
-        <v>0.0027</v>
-      </c>
-      <c r="E15" s="21">
-        <v>0.007</v>
-      </c>
-      <c r="F15" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="G15" s="21">
-        <v>1.0E-6</v>
-      </c>
-      <c r="H15" s="21">
-        <v>10000.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="20">
-        <v>0.0033</v>
-      </c>
-      <c r="D16" s="21">
-        <v>4.0E-4</v>
-      </c>
-      <c r="E16" s="21">
-        <v>4.0E-4</v>
-      </c>
-      <c r="F16" s="21">
+      <c r="G17" s="16">
         <v>3.0E-4</v>
       </c>
-      <c r="G16" s="21">
-        <v>1.0E-6</v>
-      </c>
-      <c r="H16" s="21">
-        <v>300.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="25">
-        <v>0.0026</v>
-      </c>
-      <c r="D17" s="26">
-        <v>0.0093</v>
-      </c>
-      <c r="E17" s="26">
-        <v>0.007</v>
-      </c>
-      <c r="F17" s="26">
-        <v>0.2</v>
-      </c>
-      <c r="G17" s="26">
-        <v>3.0E-4</v>
-      </c>
-      <c r="H17" s="26">
+      <c r="H17" s="16">
         <v>670.0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:G1"/>
+    <mergeCell ref="H1:H3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="H1:H3"/>
   </mergeCells>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>